<commit_message>
User creating and deleting
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Authentication, User management, Little styles, Components</t>
+  </si>
+  <si>
+    <t>Authentication implementing</t>
+  </si>
+  <si>
+    <t>User creating and deleting</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D25"/>
+  <dimension ref="B3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +451,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C564)</f>
-        <v>50.75</v>
+        <v>53.75</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -688,6 +694,28 @@
       </c>
       <c r="D25" s="1">
         <v>40857</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>40862</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>40864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User password and IsActive flag, Form permissions
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>User creating and deleting</t>
+  </si>
+  <si>
+    <t>User password and IsActive flag, Form permissions</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D27"/>
+  <dimension ref="B3:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +454,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C564)</f>
-        <v>53.75</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -716,6 +719,17 @@
       </c>
       <c r="D27" s="1">
         <v>40864</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>40865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating and editing groups
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Questions base</t>
+  </si>
+  <si>
+    <t>Creating and editing Questions</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D29"/>
+  <dimension ref="B3:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +460,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C564)</f>
-        <v>57.75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -744,6 +747,17 @@
       </c>
       <c r="D29" s="1">
         <v>40866</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>7.25</v>
+      </c>
+      <c r="D30" s="1">
+        <v>40871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Form creating, question types implementation, FormInstance creating, styles
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Creating and editing Questions</t>
+  </si>
+  <si>
+    <t>Styles, Database project</t>
+  </si>
+  <si>
+    <t>Form creating, question types implementation, FormInstance creating, styles</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D30"/>
+  <dimension ref="B3:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +466,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C564)</f>
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -758,6 +764,28 @@
       </c>
       <c r="D30" s="1">
         <v>40871</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>3.5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>40877</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>5.5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>40878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Editing Choice question, FormInstance generation and view, new window for filling
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Form creating, question types implementation, FormInstance creating, styles</t>
+  </si>
+  <si>
+    <t>Editing Choice question, FormInstance generation and view, new window for filling</t>
+  </si>
+  <si>
+    <t>Small improvements (cropping form name, …)</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D32"/>
+  <dimension ref="B3:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,8 +471,8 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
-        <f>SUM(C4:C564)</f>
-        <v>74</v>
+        <f>SUM(C4:C565)</f>
+        <v>80.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -786,6 +792,28 @@
       </c>
       <c r="D32" s="1">
         <v>40878</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>40884</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1">
+        <v>40885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing Multiline and MultipleChoice in Form edit view
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="150" windowWidth="19155" windowHeight="7965"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>Small improvements (cropping form name, …)</t>
+  </si>
+  <si>
+    <t>Meeting - Implementing Multiline and MultipleChoice questions in Form edit view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,7 +247,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +281,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,27 +456,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="104.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="C3" s="2">
         <f>SUM(C4:C565)</f>
-        <v>80.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -486,7 +487,7 @@
         <v>40823</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -497,7 +498,7 @@
         <v>40824</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -508,7 +509,7 @@
         <v>40825</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -519,7 +520,7 @@
         <v>40828</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -530,7 +531,7 @@
         <v>40830</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -541,7 +542,7 @@
         <v>40832</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -552,7 +553,7 @@
         <v>40835</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -563,7 +564,7 @@
         <v>40835</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -574,7 +575,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -585,7 +586,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -596,7 +597,7 @@
         <v>40837</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -607,7 +608,7 @@
         <v>40845</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -618,7 +619,7 @@
         <v>40845</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -629,7 +630,7 @@
         <v>40846</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -640,7 +641,7 @@
         <v>40847</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -651,7 +652,7 @@
         <v>40850</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -662,7 +663,7 @@
         <v>40851</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -673,7 +674,7 @@
         <v>40852</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -684,7 +685,7 @@
         <v>40852</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -695,7 +696,7 @@
         <v>40855</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" t="s">
         <v>19</v>
       </c>
@@ -706,7 +707,7 @@
         <v>40856</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" t="s">
         <v>20</v>
       </c>
@@ -717,7 +718,7 @@
         <v>40857</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -728,7 +729,7 @@
         <v>40862</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" t="s">
         <v>22</v>
       </c>
@@ -739,7 +740,7 @@
         <v>40864</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" t="s">
         <v>23</v>
       </c>
@@ -750,7 +751,7 @@
         <v>40865</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" t="s">
         <v>24</v>
       </c>
@@ -761,7 +762,7 @@
         <v>40866</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -772,7 +773,7 @@
         <v>40871</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -783,7 +784,7 @@
         <v>40877</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" t="s">
         <v>27</v>
       </c>
@@ -794,7 +795,7 @@
         <v>40878</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -805,7 +806,7 @@
         <v>40884</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" t="s">
         <v>28</v>
       </c>
@@ -814,6 +815,17 @@
       </c>
       <c r="D34" s="1">
         <v>40885</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>40886</v>
       </c>
     </row>
   </sheetData>
@@ -822,24 +834,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Form filling impl, styles, javascript
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Form editing - implementation, javascript, styles</t>
+  </si>
+  <si>
+    <t>Form filling - implementation, javascript, styles</t>
+  </si>
+  <si>
+    <t>Writing final report and related LaTeX learning</t>
+  </si>
+  <si>
+    <t>Writing final report, preparing presentation</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D41"/>
+  <dimension ref="B3:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +502,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C565)</f>
-        <v>100.5</v>
+        <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -912,6 +921,39 @@
       </c>
       <c r="D41" s="1">
         <v>40905</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1">
+        <v>40546</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43" s="1">
+        <v>40547</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44" s="1">
+        <v>40548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scale question, showing filled tests
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Writing final report, preparing presentation</t>
+  </si>
+  <si>
+    <t>Setting up database project, writing what to do, overview</t>
+  </si>
+  <si>
+    <t>Scale question gui and controls</t>
+  </si>
+  <si>
+    <t>Scale question, showing filled tests list and window</t>
+  </si>
+  <si>
+    <t>Showing filled tests list and window</t>
   </si>
 </sst>
 </file>
@@ -486,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D44"/>
+  <dimension ref="B3:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +514,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C565)</f>
-        <v>121.5</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -954,6 +966,50 @@
       </c>
       <c r="D44" s="1">
         <v>40548</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>40955</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>40957</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1">
+        <v>40958</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48">
+        <v>2.5</v>
+      </c>
+      <c r="D48" s="1">
+        <v>40960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
groups, permissions, TrainingTest javascript
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -148,6 +148,21 @@
   </si>
   <si>
     <t>Showing filled tests list and window</t>
+  </si>
+  <si>
+    <t>Groups, TrainingTest javascript</t>
+  </si>
+  <si>
+    <t>TrainingTest javascript &amp; styles</t>
+  </si>
+  <si>
+    <t>Groups, Permissions &amp; Managers refactoring</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Refactoring, groups</t>
   </si>
 </sst>
 </file>
@@ -498,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D48"/>
+  <dimension ref="B3:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +529,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C565)</f>
-        <v>138</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1010,6 +1025,61 @@
       </c>
       <c r="D48" s="1">
         <v>40960</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1">
+        <v>40966</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1">
+        <v>40968</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52" s="1">
+        <v>40973</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <v>1.5</v>
+      </c>
+      <c r="D53" s="1">
+        <v>40974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maximalni pocet vyplneni, mazani otazky, mazani alternativni otazky, skupiny pri editaci formu, styly, michani choice odpovedi, Google Groups csv import, vlastni obsluha vyjimek
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Cas na vyplneni - core, javascript, styles</t>
+  </si>
+  <si>
+    <t>Cas na vyplneni - zmeneno na sekundy</t>
+  </si>
+  <si>
+    <t>Maximalni pocet vyplneni, mazani otazky, mazani alternativni otazky, skupiny pri editaci formu, styly, michani choice odpovedi</t>
+  </si>
+  <si>
+    <t>Google services studium, Google Groups csv import, vlastni obsluha vyjimek</t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D57"/>
+  <dimension ref="B3:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +550,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C565)</f>
-        <v>175.5</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1136,6 +1145,39 @@
       </c>
       <c r="D57" s="1">
         <v>40981</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58">
+        <v>1.5</v>
+      </c>
+      <c r="D58" s="1">
+        <v>40983</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1">
+        <v>40986</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60" s="1">
+        <v>40987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lokalizace, export do Google Docs
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>Overovani prav na urovni Controller Actions, studium moznosti exportu do Google Docs</t>
+  </si>
+  <si>
+    <t>Michani Choice items, Lokalizace</t>
+  </si>
+  <si>
+    <t>Lokalizace, styly, Export do Google Docs</t>
+  </si>
+  <si>
+    <t>Export do CSV, Google Docs</t>
   </si>
 </sst>
 </file>
@@ -537,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D61"/>
+  <dimension ref="B3:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,8 +561,8 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
-        <f>SUM(C4:C565)</f>
-        <v>190.5</v>
+        <f>SUM(C4:C567)</f>
+        <v>199.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1192,6 +1201,39 @@
       </c>
       <c r="D61" s="1">
         <v>40988</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>40992</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63" s="1">
+        <v>40993</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>40995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FillFormReport, CSV & GoogleDocs export, TextBook, Wiki.NET parser, MarkItUp
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>Export do CSV, Google Docs</t>
+  </si>
+  <si>
+    <t>FillFormReport, Export do CSV a Google Docs</t>
+  </si>
+  <si>
+    <t>Integrace MarkItUp</t>
+  </si>
+  <si>
+    <t>Zjistovani moznosti Wiki (.net, JS), Skripta - DB, modely atd, Integrace Wiki .NET parser</t>
+  </si>
+  <si>
+    <t>Editace skript</t>
   </si>
 </sst>
 </file>
@@ -546,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D64"/>
+  <dimension ref="B3:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +574,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C567)</f>
-        <v>199.5</v>
+        <v>219.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1234,6 +1246,50 @@
       </c>
       <c r="D64" s="1">
         <v>40995</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65">
+        <v>8</v>
+      </c>
+      <c r="D65" s="1">
+        <v>40999</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>41001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>41002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bachelor (resersem, bezpecnost, ...) + makra a styly
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Finalizace UseCase, Domain a Class diagramů, řešení LaTeX obrázků, referenci, češtiny, psaní bakalářky - osnova, uvod, popis</t>
+  </si>
+  <si>
+    <t>Psaní - rešerše + screenshoty, řešení vlastních enumerací</t>
+  </si>
+  <si>
+    <t>Psaní - bezpečnost, řešení citací, řešení a  tvorba příkazů pro vkládání zdrojového kódu C#</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D70"/>
+  <dimension ref="B3:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +586,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C567)</f>
-        <v>235.5</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1318,6 +1324,28 @@
       </c>
       <c r="D70" s="1">
         <v>41006</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1">
+        <v>41007</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1">
+        <v>41008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bachelor - formulare, otazky, role
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Psaní - bezpečnost, řešení citací, řešení a  tvorba příkazů pro vkládání zdrojového kódu C#</t>
+  </si>
+  <si>
+    <t>Psaní - formulare, otazky, role, ...; reseni tabulek</t>
   </si>
 </sst>
 </file>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D72"/>
+  <dimension ref="B3:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +589,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C567)</f>
-        <v>246.5</v>
+        <v>249.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1346,6 +1349,17 @@
       </c>
       <c r="D72" s="1">
         <v>41008</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1">
+        <v>41009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bachelor - prava, ...
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -222,7 +222,7 @@
     <t>Psaní - bezpečnost, řešení citací, řešení a  tvorba příkazů pro vkládání zdrojového kódu C#</t>
   </si>
   <si>
-    <t>Psaní - formulare, otazky, role, ...; reseni tabulek</t>
+    <t>Psaní - formulare, otazky, role, prava, ...; reseni tabulek, obrazku</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="B3:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C567)</f>
-        <v>249.5</v>
+        <v>252.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>68</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D73" s="1">
         <v>41009</v>

</xml_diff>

<commit_message>
bachelor, bugs, correct/wrong answers functionality, base for unit tests
</commit_message>
<xml_diff>
--- a/project/WorkReport.xlsx
+++ b/project/WorkReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Meeting #0 - Zadani projektu</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>Selenium testy</t>
+  </si>
+  <si>
+    <t>Selenium na notebooku, konzultace, mensi upravy</t>
+  </si>
+  <si>
+    <t>Unit testy, psani</t>
+  </si>
+  <si>
+    <t>Psani, bugy, dodelani funkcionality, tvorba pilotnich testu</t>
   </si>
 </sst>
 </file>
@@ -607,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D89"/>
+  <dimension ref="B3:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +632,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f>SUM(C4:C567)</f>
-        <v>339.5</v>
+        <v>375.5</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1567,6 +1576,61 @@
       </c>
       <c r="D89" s="1">
         <v>41043</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>80</v>
+      </c>
+      <c r="C90" s="3">
+        <v>4</v>
+      </c>
+      <c r="D90" s="1">
+        <v>41044</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="3">
+        <v>5</v>
+      </c>
+      <c r="D91" s="1">
+        <v>41045</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>77</v>
+      </c>
+      <c r="C92" s="3">
+        <v>9</v>
+      </c>
+      <c r="D92" s="1">
+        <v>41046</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" s="3">
+        <v>7</v>
+      </c>
+      <c r="D93" s="1">
+        <v>41048</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="3">
+        <v>11</v>
+      </c>
+      <c r="D94" s="1">
+        <v>41049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>